<commit_message>
Update DataSheet for the conflicts
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set_EU.xlsx
+++ b/DataSet/Integration_DataSet/CommSee/COMMSEE_Data_Set_EU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u723925\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\CommSee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93EB9BE-B5F4-4C7F-81AB-45937A830453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A35DCA-3679-449B-9B9E-B5CAD85612D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" firstSheet="36" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" firstSheet="35" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9864" uniqueCount="1651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9883" uniqueCount="1651">
   <si>
     <t>@</t>
   </si>
@@ -5380,7 +5380,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5731,45 +5731,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -21415,7 +21394,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="CY1" activePane="topRight" state="frozen"/>
       <selection activeCell="CV15" sqref="CV15"/>
-      <selection pane="topRight" activeCell="CR7" sqref="CR7"/>
+      <selection pane="topRight" activeCell="CX6" sqref="CX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23110,29 +23089,29 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="6" spans="1:106" s="221" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A6" s="145">
         <v>5</v>
       </c>
-      <c r="B6" s="212" t="s">
+      <c r="B6" s="209" t="s">
         <v>1324</v>
       </c>
-      <c r="C6" s="145">
+      <c r="C6" s="195">
         <v>3000665</v>
       </c>
-      <c r="D6" s="212" t="s">
+      <c r="D6" s="209" t="s">
         <v>481</v>
       </c>
-      <c r="E6" s="212" t="s">
+      <c r="E6" s="209" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="212" t="s">
+      <c r="F6" s="209" t="s">
         <v>174</v>
       </c>
       <c r="G6" s="213">
         <v>43750</v>
       </c>
-      <c r="H6" s="145" t="s">
+      <c r="H6" s="195" t="s">
         <v>1645</v>
       </c>
       <c r="I6" s="145">
@@ -23141,288 +23120,288 @@
       <c r="J6" s="213">
         <v>44138</v>
       </c>
-      <c r="K6" s="145">
-        <v>100000</v>
-      </c>
-      <c r="L6" s="212" t="s">
+      <c r="K6" s="170" t="s">
+        <v>489</v>
+      </c>
+      <c r="L6" s="209" t="s">
         <v>98</v>
       </c>
-      <c r="M6" s="145" t="s">
+      <c r="M6" s="195" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="145" t="s">
+      <c r="N6" s="195" t="s">
         <v>490</v>
       </c>
-      <c r="O6" s="214" t="s">
+      <c r="O6" s="210" t="s">
         <v>102</v>
       </c>
-      <c r="P6" s="145" t="s">
+      <c r="P6" s="195" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" s="222">
+      <c r="Q6" s="195">
         <v>1</v>
       </c>
-      <c r="R6" s="222">
+      <c r="R6" s="195">
         <v>1</v>
       </c>
-      <c r="S6" s="222">
+      <c r="S6" s="195">
         <v>3</v>
       </c>
-      <c r="T6" s="145">
-        <v>100000</v>
-      </c>
-      <c r="U6" s="145">
-        <v>100000</v>
-      </c>
-      <c r="V6" s="145">
-        <v>100000</v>
-      </c>
-      <c r="W6" s="145" t="s">
+      <c r="T6" s="170" t="s">
+        <v>489</v>
+      </c>
+      <c r="U6" s="170" t="s">
+        <v>489</v>
+      </c>
+      <c r="V6" s="170" t="s">
+        <v>489</v>
+      </c>
+      <c r="W6" s="195" t="s">
         <v>106</v>
       </c>
-      <c r="X6" s="214" t="s">
+      <c r="X6" s="210" t="s">
         <v>107</v>
       </c>
-      <c r="Y6" s="145" t="s">
+      <c r="Y6" s="195" t="s">
         <v>1330</v>
       </c>
-      <c r="Z6" s="145" t="s">
+      <c r="Z6" s="195" t="s">
         <v>1331</v>
       </c>
-      <c r="AA6" s="145" t="s">
+      <c r="AA6" s="195" t="s">
         <v>1332</v>
       </c>
-      <c r="AB6" s="145" t="s">
+      <c r="AB6" s="195" t="s">
         <v>1646</v>
       </c>
-      <c r="AC6" s="214" t="s">
+      <c r="AC6" s="210" t="s">
         <v>493</v>
       </c>
-      <c r="AD6" s="145" t="s">
+      <c r="AD6" s="195" t="s">
         <v>494</v>
       </c>
-      <c r="AE6" s="145" t="s">
+      <c r="AE6" s="195" t="s">
         <v>495</v>
       </c>
-      <c r="AF6" s="214" t="s">
+      <c r="AF6" s="210" t="s">
         <v>496</v>
       </c>
-      <c r="AG6" s="214" t="s">
+      <c r="AG6" s="210" t="s">
         <v>497</v>
       </c>
-      <c r="AH6" s="214" t="s">
+      <c r="AH6" s="210" t="s">
         <v>498</v>
       </c>
-      <c r="AI6" s="214" t="s">
+      <c r="AI6" s="210" t="s">
         <v>499</v>
       </c>
-      <c r="AJ6" s="214" t="s">
+      <c r="AJ6" s="210" t="s">
         <v>495</v>
       </c>
-      <c r="AK6" s="214" t="s">
+      <c r="AK6" s="210" t="s">
         <v>500</v>
       </c>
-      <c r="AL6" s="214" t="s">
+      <c r="AL6" s="210" t="s">
         <v>1334</v>
       </c>
-      <c r="AM6" s="214" t="s">
+      <c r="AM6" s="210" t="s">
         <v>501</v>
       </c>
-      <c r="AN6" s="214" t="s">
+      <c r="AN6" s="210" t="s">
         <v>502</v>
       </c>
-      <c r="AO6" s="215">
-        <v>10000000</v>
-      </c>
-      <c r="AP6" s="214" t="s">
+      <c r="AO6" s="173" t="s">
+        <v>503</v>
+      </c>
+      <c r="AP6" s="210" t="s">
         <v>495</v>
       </c>
-      <c r="AQ6" s="214" t="s">
+      <c r="AQ6" s="210" t="s">
         <v>230</v>
       </c>
-      <c r="AR6" s="214" t="s">
+      <c r="AR6" s="210" t="s">
         <v>98</v>
       </c>
-      <c r="AS6" s="214" t="s">
+      <c r="AS6" s="210" t="s">
         <v>504</v>
       </c>
-      <c r="AT6" s="214" t="s">
+      <c r="AT6" s="210" t="s">
         <v>504</v>
       </c>
-      <c r="AU6" s="214" t="s">
+      <c r="AU6" s="210" t="s">
         <v>505</v>
       </c>
-      <c r="AV6" s="214" t="s">
+      <c r="AV6" s="210" t="s">
         <v>506</v>
       </c>
-      <c r="AW6" s="145" t="s">
+      <c r="AW6" s="195" t="s">
         <v>507</v>
       </c>
-      <c r="AX6" s="222">
+      <c r="AX6" s="195">
         <v>2</v>
       </c>
-      <c r="AY6" s="214" t="s">
+      <c r="AY6" s="210" t="s">
         <v>372</v>
       </c>
-      <c r="AZ6" s="214" t="s">
+      <c r="AZ6" s="210" t="s">
         <v>508</v>
       </c>
-      <c r="BA6" s="214" t="s">
+      <c r="BA6" s="210" t="s">
         <v>505</v>
       </c>
-      <c r="BB6" s="222">
+      <c r="BB6" s="195">
         <v>2</v>
       </c>
-      <c r="BC6" s="145" t="s">
+      <c r="BC6" s="195" t="s">
         <v>509</v>
       </c>
-      <c r="BD6" s="214" t="s">
+      <c r="BD6" s="210" t="s">
         <v>499</v>
       </c>
-      <c r="BE6" s="214" t="s">
+      <c r="BE6" s="210" t="s">
         <v>495</v>
       </c>
-      <c r="BF6" s="214" t="s">
+      <c r="BF6" s="210" t="s">
         <v>510</v>
       </c>
-      <c r="BG6" s="145" t="s">
+      <c r="BG6" s="195" t="s">
         <v>511</v>
       </c>
-      <c r="BH6" s="222">
+      <c r="BH6" s="195">
         <v>100</v>
       </c>
-      <c r="BI6" s="222">
+      <c r="BI6" s="195">
         <v>100</v>
       </c>
-      <c r="BJ6" s="145" t="s">
+      <c r="BJ6" s="195" t="s">
         <v>1191</v>
       </c>
-      <c r="BK6" s="214" t="s">
+      <c r="BK6" s="210" t="s">
         <v>513</v>
       </c>
-      <c r="BL6" s="145" t="s">
+      <c r="BL6" s="195" t="s">
         <v>514</v>
       </c>
-      <c r="BM6" s="214" t="s">
+      <c r="BM6" s="210" t="s">
         <v>515</v>
       </c>
-      <c r="BN6" s="214" t="s">
+      <c r="BN6" s="210" t="s">
         <v>516</v>
       </c>
-      <c r="BO6" s="215">
-        <v>100000</v>
-      </c>
-      <c r="BP6" s="214">
-        <v>100</v>
-      </c>
-      <c r="BQ6" s="216">
+      <c r="BO6" s="173" t="s">
+        <v>517</v>
+      </c>
+      <c r="BP6" s="173" t="s">
+        <v>1066</v>
+      </c>
+      <c r="BQ6" s="214">
         <v>44503</v>
       </c>
-      <c r="BR6" s="216">
+      <c r="BR6" s="214">
         <v>43461</v>
       </c>
-      <c r="BS6" s="145"/>
-      <c r="BT6" s="217" t="s">
+      <c r="BS6" s="195"/>
+      <c r="BT6" s="211" t="s">
         <v>516</v>
       </c>
-      <c r="BU6" s="218">
-        <v>100000</v>
-      </c>
-      <c r="BV6" s="217" t="s">
+      <c r="BU6" s="177" t="s">
+        <v>517</v>
+      </c>
+      <c r="BV6" s="211" t="s">
         <v>98</v>
       </c>
-      <c r="BW6" s="217" t="s">
+      <c r="BW6" s="211" t="s">
         <v>700</v>
       </c>
-      <c r="BX6" s="217" t="s">
+      <c r="BX6" s="211" t="s">
         <v>566</v>
       </c>
-      <c r="BY6" s="217" t="s">
+      <c r="BY6" s="211" t="s">
         <v>566</v>
       </c>
-      <c r="BZ6" s="219">
-        <v>1</v>
-      </c>
-      <c r="CA6" s="217" t="s">
+      <c r="BZ6" s="177" t="s">
+        <v>568</v>
+      </c>
+      <c r="CA6" s="211" t="s">
         <v>1348</v>
       </c>
-      <c r="CB6" s="220" t="s">
+      <c r="CB6" s="212" t="s">
         <v>1647</v>
       </c>
-      <c r="CC6" s="217" t="s">
+      <c r="CC6" s="211" t="s">
         <v>702</v>
       </c>
-      <c r="CD6" s="220" t="s">
+      <c r="CD6" s="212" t="s">
         <v>1648</v>
       </c>
-      <c r="CE6" s="217" t="s">
+      <c r="CE6" s="211" t="s">
         <v>702</v>
       </c>
-      <c r="CF6" s="220" t="s">
+      <c r="CF6" s="212" t="s">
         <v>1649</v>
       </c>
-      <c r="CG6" s="220" t="s">
+      <c r="CG6" s="212" t="s">
         <v>702</v>
       </c>
-      <c r="CH6" s="216">
+      <c r="CH6" s="214">
         <v>43461</v>
       </c>
-      <c r="CI6" s="216">
+      <c r="CI6" s="214">
         <v>43461</v>
       </c>
-      <c r="CJ6" s="217" t="s">
+      <c r="CJ6" s="211" t="s">
         <v>1341</v>
       </c>
-      <c r="CK6" s="217" t="s">
+      <c r="CK6" s="211" t="s">
         <v>516</v>
       </c>
-      <c r="CL6" s="217" t="s">
+      <c r="CL6" s="211" t="s">
         <v>520</v>
       </c>
-      <c r="CM6" s="217" t="s">
+      <c r="CM6" s="211" t="s">
         <v>504</v>
       </c>
-      <c r="CN6" s="217" t="s">
+      <c r="CN6" s="211" t="s">
         <v>504</v>
       </c>
-      <c r="CO6" s="217" t="s">
+      <c r="CO6" s="211" t="s">
         <v>505</v>
       </c>
-      <c r="CP6" s="217" t="s">
+      <c r="CP6" s="211" t="s">
         <v>98</v>
       </c>
-      <c r="CQ6" s="217">
-        <v>2</v>
-      </c>
-      <c r="CR6" s="217" t="s">
+      <c r="CQ6" s="177" t="s">
+        <v>118</v>
+      </c>
+      <c r="CR6" s="211" t="s">
         <v>521</v>
       </c>
-      <c r="CS6" s="217" t="s">
+      <c r="CS6" s="211" t="s">
         <v>522</v>
       </c>
-      <c r="CT6" s="217" t="s">
+      <c r="CT6" s="211" t="s">
         <v>502</v>
       </c>
-      <c r="CU6" s="216">
+      <c r="CU6" s="214">
         <v>43461</v>
       </c>
-      <c r="CV6" s="216">
+      <c r="CV6" s="214">
         <v>43461</v>
       </c>
-      <c r="CW6" s="145"/>
-      <c r="CX6" s="216">
+      <c r="CW6" s="195"/>
+      <c r="CX6" s="214">
         <v>43461</v>
       </c>
-      <c r="CY6" s="217" t="s">
+      <c r="CY6" s="211" t="s">
         <v>533</v>
       </c>
-      <c r="CZ6" s="217" t="s">
+      <c r="CZ6" s="211" t="s">
         <v>511</v>
       </c>
-      <c r="DA6" s="217" t="s">
+      <c r="DA6" s="211" t="s">
         <v>499</v>
       </c>
-      <c r="DB6" s="217" t="s">
+      <c r="DB6" s="211" t="s">
         <v>516</v>
       </c>
     </row>
@@ -23760,7 +23739,7 @@
       <selection activeCell="CV15" sqref="CV15"/>
       <selection pane="topRight" activeCell="CV15" sqref="CV15"/>
       <selection pane="bottomLeft" activeCell="CV15" sqref="CV15"/>
-      <selection pane="bottomRight" activeCell="AY12" sqref="AY12"/>
+      <selection pane="bottomRight" activeCell="AY6" sqref="AY6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -24557,7 +24536,7 @@
       </c>
     </row>
     <row r="6" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="145">
+      <c r="A6" s="195">
         <v>5</v>
       </c>
       <c r="B6" s="209" t="s">
@@ -24584,8 +24563,8 @@
       <c r="I6" s="195" t="s">
         <v>184</v>
       </c>
-      <c r="J6" s="145">
-        <v>100000</v>
+      <c r="J6" s="170" t="s">
+        <v>489</v>
       </c>
       <c r="K6" s="145">
         <v>10000</v>
@@ -24611,17 +24590,17 @@
       <c r="R6" s="195">
         <v>1</v>
       </c>
-      <c r="S6" s="145">
-        <v>100000</v>
-      </c>
-      <c r="T6" s="145">
-        <v>100000</v>
-      </c>
-      <c r="U6" s="145">
-        <v>100000</v>
-      </c>
-      <c r="V6" s="145">
-        <v>10000</v>
+      <c r="S6" s="170" t="s">
+        <v>489</v>
+      </c>
+      <c r="T6" s="170" t="s">
+        <v>489</v>
+      </c>
+      <c r="U6" s="170" t="s">
+        <v>489</v>
+      </c>
+      <c r="V6" s="170" t="s">
+        <v>489</v>
       </c>
       <c r="W6" s="145">
         <v>90000</v>
@@ -24659,17 +24638,17 @@
       <c r="AH6" s="210" t="s">
         <v>98</v>
       </c>
-      <c r="AI6" s="215">
-        <v>100000</v>
+      <c r="AI6" s="184" t="s">
+        <v>517</v>
       </c>
       <c r="AJ6" s="195"/>
-      <c r="AK6" s="216">
+      <c r="AK6" s="214">
         <v>43461</v>
       </c>
-      <c r="AL6" s="216">
+      <c r="AL6" s="214">
         <v>43693</v>
       </c>
-      <c r="AM6" s="216">
+      <c r="AM6" s="214">
         <v>43723</v>
       </c>
       <c r="AN6" s="210" t="s">
@@ -24934,7 +24913,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AR6" sqref="AR6"/>
+      <selection pane="bottomRight" activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -25599,7 +25578,7 @@
       <c r="E6" s="145">
         <v>3000665</v>
       </c>
-      <c r="F6" s="170" t="s">
+      <c r="F6" s="217" t="s">
         <v>1028</v>
       </c>
       <c r="G6" s="195" t="s">
@@ -25638,14 +25617,14 @@
       <c r="R6" s="213">
         <v>44229</v>
       </c>
-      <c r="S6" s="145">
-        <v>0</v>
-      </c>
-      <c r="T6" s="137">
-        <v>0</v>
-      </c>
-      <c r="U6" s="145">
-        <v>0</v>
+      <c r="S6" s="170" t="s">
+        <v>559</v>
+      </c>
+      <c r="T6" s="170" t="s">
+        <v>559</v>
+      </c>
+      <c r="U6" s="170" t="s">
+        <v>559</v>
       </c>
       <c r="V6" s="195" t="s">
         <v>1646</v>
@@ -25656,7 +25635,7 @@
       <c r="X6" s="210" t="s">
         <v>372</v>
       </c>
-      <c r="Y6" s="223" t="s">
+      <c r="Y6" s="215" t="s">
         <v>588</v>
       </c>
       <c r="Z6" s="210" t="s">
@@ -25683,7 +25662,7 @@
       <c r="AG6" s="210" t="s">
         <v>230</v>
       </c>
-      <c r="AH6" s="224" t="s">
+      <c r="AH6" s="216" t="s">
         <v>588</v>
       </c>
       <c r="AI6" s="210" t="s">
@@ -25912,8 +25891,8 @@
   </sheetPr>
   <dimension ref="A1:DB7"/>
   <sheetViews>
-    <sheetView topLeftCell="BI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN29" sqref="BN29"/>
+    <sheetView topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BN6" sqref="BN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26765,7 +26744,7 @@
       </c>
     </row>
     <row r="6" spans="1:106" x14ac:dyDescent="0.3">
-      <c r="A6" s="225">
+      <c r="A6" s="218">
         <v>5</v>
       </c>
       <c r="B6" s="209" t="s">
@@ -26780,7 +26759,7 @@
       <c r="E6" s="145">
         <v>3000665</v>
       </c>
-      <c r="F6" s="226" t="s">
+      <c r="F6" s="219" t="s">
         <v>1028</v>
       </c>
       <c r="G6" s="195" t="s">
@@ -26855,13 +26834,13 @@
       <c r="AD6" s="206" t="s">
         <v>1066</v>
       </c>
-      <c r="AE6" s="216">
+      <c r="AE6" s="214">
         <v>43461</v>
       </c>
       <c r="AF6" s="213">
         <v>44138</v>
       </c>
-      <c r="AG6" s="216">
+      <c r="AG6" s="214">
         <v>44533</v>
       </c>
       <c r="AH6" s="213">
@@ -26888,7 +26867,7 @@
       <c r="AO6" s="206" t="s">
         <v>87</v>
       </c>
-      <c r="AP6" s="216">
+      <c r="AP6" s="214">
         <v>43461</v>
       </c>
       <c r="AQ6" s="211" t="s">
@@ -27202,9 +27181,9 @@
   </sheetPr>
   <dimension ref="A1:DB7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27584,7 +27563,7 @@
       </c>
     </row>
     <row r="6" spans="1:106" x14ac:dyDescent="0.3">
-      <c r="A6" s="225">
+      <c r="A6" s="218">
         <v>5</v>
       </c>
       <c r="B6" s="209" t="s">
@@ -27623,7 +27602,7 @@
       <c r="M6" s="76" t="s">
         <v>1438</v>
       </c>
-      <c r="N6" s="195">
+      <c r="N6" s="67">
         <v>100</v>
       </c>
       <c r="O6" s="195" t="s">
@@ -27782,8 +27761,8 @@
   </sheetPr>
   <dimension ref="A1:DB8"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28120,149 +28099,149 @@
       <c r="A6" s="145">
         <v>5</v>
       </c>
-      <c r="B6" s="209" t="s">
+      <c r="B6" s="220" t="s">
         <v>1324</v>
       </c>
-      <c r="C6" s="195" t="s">
+      <c r="C6" s="145" t="s">
         <v>1645</v>
       </c>
-      <c r="D6" s="195" t="s">
+      <c r="D6" s="145" t="s">
         <v>1646</v>
       </c>
       <c r="E6" s="145">
         <v>60000762</v>
       </c>
-      <c r="F6" s="216">
+      <c r="F6" s="214">
         <v>44145</v>
       </c>
-      <c r="G6" s="211" t="s">
+      <c r="G6" s="221" t="s">
         <v>1445</v>
       </c>
-      <c r="H6" s="195" t="s">
+      <c r="H6" s="145" t="s">
         <v>861</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="195" t="s">
+      <c r="J6" s="145" t="s">
         <v>1446</v>
       </c>
       <c r="K6" s="195" t="s">
         <v>1447</v>
       </c>
-      <c r="L6" s="195" t="s">
+      <c r="L6" s="145" t="s">
         <v>227</v>
       </c>
-      <c r="M6" s="195" t="s">
+      <c r="M6" s="145" t="s">
         <v>1448</v>
       </c>
-      <c r="N6" s="195" t="s">
+      <c r="N6" s="145" t="s">
         <v>817</v>
       </c>
-      <c r="O6" s="195" t="s">
+      <c r="O6" s="145" t="s">
         <v>1449</v>
       </c>
-      <c r="P6" s="211" t="s">
+      <c r="P6" s="221" t="s">
         <v>675</v>
       </c>
-      <c r="Q6" s="195" t="s">
+      <c r="Q6" s="145" t="s">
         <v>1313</v>
       </c>
-      <c r="R6" s="195">
+      <c r="R6" s="67">
         <v>100</v>
       </c>
-      <c r="S6" s="195" t="s">
+      <c r="S6" s="145" t="s">
         <v>1490</v>
       </c>
-      <c r="T6" s="195" t="s">
+      <c r="T6" s="145" t="s">
         <v>1450</v>
       </c>
-      <c r="U6" s="211"/>
-      <c r="V6" s="211"/>
-      <c r="W6" s="211"/>
-      <c r="X6" s="211"/>
-      <c r="Y6" s="211"/>
-      <c r="Z6" s="211"/>
-      <c r="AA6" s="211"/>
-      <c r="AB6" s="211"/>
-      <c r="AC6" s="211"/>
-      <c r="AD6" s="211"/>
-      <c r="AE6" s="211"/>
-      <c r="AF6" s="211"/>
-      <c r="AG6" s="211"/>
-      <c r="AH6" s="211"/>
-      <c r="AI6" s="211"/>
-      <c r="AJ6" s="211"/>
-      <c r="AK6" s="211"/>
-      <c r="AL6" s="211"/>
-      <c r="AM6" s="211"/>
-      <c r="AN6" s="211"/>
-      <c r="AO6" s="211"/>
-      <c r="AP6" s="211"/>
-      <c r="AQ6" s="211"/>
-      <c r="AR6" s="211"/>
-      <c r="AS6" s="211"/>
-      <c r="AT6" s="211"/>
-      <c r="AU6" s="211"/>
-      <c r="AV6" s="211"/>
-      <c r="AW6" s="211"/>
-      <c r="AX6" s="211"/>
-      <c r="AY6" s="211"/>
-      <c r="AZ6" s="211"/>
-      <c r="BA6" s="211"/>
-      <c r="BB6" s="211"/>
-      <c r="BC6" s="211"/>
-      <c r="BD6" s="211"/>
-      <c r="BE6" s="211"/>
-      <c r="BF6" s="211"/>
-      <c r="BG6" s="211"/>
-      <c r="BH6" s="211"/>
-      <c r="BI6" s="211"/>
-      <c r="BJ6" s="211"/>
-      <c r="BK6" s="211"/>
-      <c r="BL6" s="211"/>
-      <c r="BM6" s="211"/>
-      <c r="BN6" s="211"/>
-      <c r="BO6" s="211"/>
-      <c r="BP6" s="211"/>
-      <c r="BQ6" s="211"/>
-      <c r="BR6" s="211"/>
-      <c r="BS6" s="211"/>
-      <c r="BT6" s="211"/>
-      <c r="BU6" s="211"/>
-      <c r="BV6" s="211"/>
-      <c r="BW6" s="211"/>
-      <c r="BX6" s="211"/>
-      <c r="BY6" s="211"/>
-      <c r="BZ6" s="211"/>
-      <c r="CA6" s="211"/>
-      <c r="CB6" s="211"/>
-      <c r="CC6" s="211"/>
-      <c r="CD6" s="211"/>
-      <c r="CE6" s="211"/>
-      <c r="CF6" s="211"/>
-      <c r="CG6" s="211"/>
-      <c r="CH6" s="211"/>
-      <c r="CI6" s="211"/>
-      <c r="CJ6" s="211"/>
-      <c r="CK6" s="211"/>
-      <c r="CL6" s="211"/>
-      <c r="CM6" s="211"/>
-      <c r="CN6" s="211"/>
-      <c r="CO6" s="211"/>
-      <c r="CP6" s="211"/>
-      <c r="CQ6" s="211"/>
-      <c r="CR6" s="211"/>
-      <c r="CS6" s="211"/>
-      <c r="CT6" s="211"/>
-      <c r="CU6" s="211"/>
-      <c r="CV6" s="211"/>
-      <c r="CW6" s="211"/>
-      <c r="CX6" s="211"/>
-      <c r="CY6" s="211"/>
-      <c r="CZ6" s="211"/>
-      <c r="DA6" s="211"/>
-      <c r="DB6" s="211"/>
+      <c r="U6" s="221"/>
+      <c r="V6" s="221"/>
+      <c r="W6" s="221"/>
+      <c r="X6" s="221"/>
+      <c r="Y6" s="221"/>
+      <c r="Z6" s="221"/>
+      <c r="AA6" s="221"/>
+      <c r="AB6" s="221"/>
+      <c r="AC6" s="221"/>
+      <c r="AD6" s="221"/>
+      <c r="AE6" s="221"/>
+      <c r="AF6" s="221"/>
+      <c r="AG6" s="221"/>
+      <c r="AH6" s="221"/>
+      <c r="AI6" s="221"/>
+      <c r="AJ6" s="221"/>
+      <c r="AK6" s="221"/>
+      <c r="AL6" s="221"/>
+      <c r="AM6" s="221"/>
+      <c r="AN6" s="221"/>
+      <c r="AO6" s="221"/>
+      <c r="AP6" s="221"/>
+      <c r="AQ6" s="221"/>
+      <c r="AR6" s="221"/>
+      <c r="AS6" s="221"/>
+      <c r="AT6" s="221"/>
+      <c r="AU6" s="221"/>
+      <c r="AV6" s="221"/>
+      <c r="AW6" s="221"/>
+      <c r="AX6" s="221"/>
+      <c r="AY6" s="221"/>
+      <c r="AZ6" s="221"/>
+      <c r="BA6" s="221"/>
+      <c r="BB6" s="221"/>
+      <c r="BC6" s="221"/>
+      <c r="BD6" s="221"/>
+      <c r="BE6" s="221"/>
+      <c r="BF6" s="221"/>
+      <c r="BG6" s="221"/>
+      <c r="BH6" s="221"/>
+      <c r="BI6" s="221"/>
+      <c r="BJ6" s="221"/>
+      <c r="BK6" s="221"/>
+      <c r="BL6" s="221"/>
+      <c r="BM6" s="221"/>
+      <c r="BN6" s="221"/>
+      <c r="BO6" s="221"/>
+      <c r="BP6" s="221"/>
+      <c r="BQ6" s="221"/>
+      <c r="BR6" s="221"/>
+      <c r="BS6" s="221"/>
+      <c r="BT6" s="221"/>
+      <c r="BU6" s="221"/>
+      <c r="BV6" s="221"/>
+      <c r="BW6" s="221"/>
+      <c r="BX6" s="221"/>
+      <c r="BY6" s="221"/>
+      <c r="BZ6" s="221"/>
+      <c r="CA6" s="221"/>
+      <c r="CB6" s="221"/>
+      <c r="CC6" s="221"/>
+      <c r="CD6" s="221"/>
+      <c r="CE6" s="221"/>
+      <c r="CF6" s="221"/>
+      <c r="CG6" s="221"/>
+      <c r="CH6" s="221"/>
+      <c r="CI6" s="221"/>
+      <c r="CJ6" s="221"/>
+      <c r="CK6" s="221"/>
+      <c r="CL6" s="221"/>
+      <c r="CM6" s="221"/>
+      <c r="CN6" s="221"/>
+      <c r="CO6" s="221"/>
+      <c r="CP6" s="221"/>
+      <c r="CQ6" s="221"/>
+      <c r="CR6" s="221"/>
+      <c r="CS6" s="221"/>
+      <c r="CT6" s="221"/>
+      <c r="CU6" s="221"/>
+      <c r="CV6" s="221"/>
+      <c r="CW6" s="221"/>
+      <c r="CX6" s="221"/>
+      <c r="CY6" s="221"/>
+      <c r="CZ6" s="221"/>
+      <c r="DA6" s="221"/>
+      <c r="DB6" s="221"/>
     </row>
     <row r="7" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A7" s="193" t="s">
@@ -28789,8 +28768,8 @@
   <dimension ref="A1:DB7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -29280,16 +29259,16 @@
       </c>
     </row>
     <row r="6" spans="1:106" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="225">
+      <c r="A6" s="218">
         <v>5</v>
       </c>
       <c r="B6" s="209" t="s">
         <v>1324</v>
       </c>
-      <c r="C6" s="216">
+      <c r="C6" s="196">
         <v>44115</v>
       </c>
-      <c r="D6" s="216">
+      <c r="D6" s="196">
         <v>44175</v>
       </c>
       <c r="E6" s="210" t="s">
@@ -29340,10 +29319,10 @@
       <c r="T6" s="195" t="s">
         <v>1491</v>
       </c>
-      <c r="U6" s="216">
+      <c r="U6" s="214">
         <v>44138</v>
       </c>
-      <c r="V6" s="216">
+      <c r="V6" s="214">
         <v>43255</v>
       </c>
       <c r="W6" s="195" t="s">
@@ -29365,7 +29344,7 @@
       <c r="AC6" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="AD6" s="216">
+      <c r="AD6" s="214">
         <v>44145</v>
       </c>
       <c r="AF6" s="211"/>

</xml_diff>